<commit_message>
chore: update data outputs, frontend components, scripts and tests
</commit_message>
<xml_diff>
--- a/data/01_raw/SEDE+regic.xlsx
+++ b/data/01_raw/SEDE+regic.xlsx
@@ -2681,8 +2681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G752"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A750" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C756" sqref="C756"/>
+    <sheetView tabSelected="1" topLeftCell="A738" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D753" sqref="D753"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13166,6 +13166,7 @@
       <c r="D748" t="s">
         <v>763</v>
       </c>
+      <c r="G748" s="1"/>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A749">

</xml_diff>